<commit_message>
feat: Implement evaluation and session models with MongoDB integration
</commit_message>
<xml_diff>
--- a/data/system_B_response_from_db.xlsx
+++ b/data/system_B_response_from_db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data fetching scrypt\System_B_Response\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data fetching scrypt\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D981FF0-0EC2-45D1-B200-D22194561AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2254C218-D1AC-449C-893C-2743AB605D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -400,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -410,6 +410,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,21 +718,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="26.33203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="36.88671875" style="1" customWidth="1"/>
     <col min="5" max="5" width="53" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="54" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -746,11 +749,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -763,11 +766,11 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="187.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -781,10 +784,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -798,10 +801,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -815,10 +818,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">

</xml_diff>